<commit_message>
dot env y otros
</commit_message>
<xml_diff>
--- a/excel/PEDIDO YA CON VENDEDOR.xlsx
+++ b/excel/PEDIDO YA CON VENDEDOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\$ Gustavo\3. Programación\3.2. Proyectos\3.2.10. Megamoto-Campaña WhatsApp\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D678B06-1258-4B07-B9B7-5AC016FC25A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA54B2D-0550-421B-9579-46A6E6EEA5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
     <t>VENDEDOR</t>
   </si>
   <si>
-    <t>GUSTAVO GLUNZ</t>
+    <t>GUSTAVO</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -369,7 +369,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>5491159911742</v>
+        <v>5491161405589</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -378,7 +378,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <v>5491159911742</v>
+        <v>5491161405589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>